<commit_message>
Agregado las distancias de cada punto, archivos reorganizados y prueba exitosa del funcionamiento
</commit_message>
<xml_diff>
--- a/output/joined_data.xlsx
+++ b/output/joined_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,16 @@
           <t>elevacion</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>distancia</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>distancia_acumulada</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -494,6 +504,12 @@
       <c r="G2" t="n">
         <v>3811.70751953125</v>
       </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -519,6 +535,12 @@
       <c r="G3" t="n">
         <v>3811.9892578125</v>
       </c>
+      <c r="H3" t="n">
+        <v>72.34634270106764</v>
+      </c>
+      <c r="I3" t="n">
+        <v>72.34634270106764</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -544,6 +566,12 @@
       <c r="G4" t="n">
         <v>3811.9072265625</v>
       </c>
+      <c r="H4" t="n">
+        <v>45.80919622254626</v>
+      </c>
+      <c r="I4" t="n">
+        <v>118.1555389236139</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -569,6 +597,12 @@
       <c r="G5" t="n">
         <v>3807.909912109375</v>
       </c>
+      <c r="H5" t="n">
+        <v>47.94858565865728</v>
+      </c>
+      <c r="I5" t="n">
+        <v>166.1041245822712</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -594,6 +628,12 @@
       <c r="G6" t="n">
         <v>3806.519775390625</v>
       </c>
+      <c r="H6" t="n">
+        <v>53.98061808053652</v>
+      </c>
+      <c r="I6" t="n">
+        <v>220.0847426628077</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -619,6 +659,12 @@
       <c r="G7" t="n">
         <v>3808.522216796875</v>
       </c>
+      <c r="H7" t="n">
+        <v>59.08065155388351</v>
+      </c>
+      <c r="I7" t="n">
+        <v>279.1653942166912</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -644,19 +690,25 @@
       <c r="G8" t="n">
         <v>3818.451416015625</v>
       </c>
+      <c r="H8" t="n">
+        <v>37.15268647337687</v>
+      </c>
+      <c r="I8" t="n">
+        <v>316.3180806900681</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-71.5051914121306</v>
+        <v>-71.50511592146341</v>
       </c>
       <c r="B9" t="n">
-        <v>-15.52551596548126</v>
+        <v>-15.5254870799914</v>
       </c>
       <c r="C9" t="n">
-        <v>231268.3864369696</v>
+        <v>231276.4513187492</v>
       </c>
       <c r="D9" t="n">
-        <v>8281974.986131702</v>
+        <v>8281978.278665429</v>
       </c>
       <c r="E9" t="n">
         <v>19</v>
@@ -667,7 +719,13 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>3828.814453125</v>
+        <v>3829.822998046875</v>
+      </c>
+      <c r="H9" t="n">
+        <v>33.21617207162281</v>
+      </c>
+      <c r="I9" t="n">
+        <v>349.5342527616909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>